<commit_message>
Add "mex" mission elements to spreadsheet
</commit_message>
<xml_diff>
--- a/PD2 Scripts.xlsx
+++ b/PD2 Scripts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Users\JiN\Documents\Ohjelmointia\PD2 Modit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ohjelmointi\Modit\PD2 Mod - Forced RNG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E3D75A5A-D582-4AC9-A1D1-34D6782BF532}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509FF4E2-2BCB-4E1B-A81D-4F60B9FF5757}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12585" tabRatio="717" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="717" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Misc." sheetId="12" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9299" uniqueCount="4284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9368" uniqueCount="4307">
   <si>
     <t>Art Gallery</t>
   </si>
@@ -15836,6 +15836,75 @@
   </si>
   <si>
     <t>100343</t>
+  </si>
+  <si>
+    <t>100708</t>
+  </si>
+  <si>
+    <t>random_mandatory_loot</t>
+  </si>
+  <si>
+    <t>loot_is_weapons</t>
+  </si>
+  <si>
+    <t>Weapons</t>
+  </si>
+  <si>
+    <t>100710</t>
+  </si>
+  <si>
+    <t>loot_is_money</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>loot_is_coke</t>
+  </si>
+  <si>
+    <t>Coke</t>
+  </si>
+  <si>
+    <t>102007</t>
+  </si>
+  <si>
+    <t>random_camera_room</t>
+  </si>
+  <si>
+    <t>Random security room</t>
+  </si>
+  <si>
+    <t>102009</t>
+  </si>
+  <si>
+    <t>102010</t>
+  </si>
+  <si>
+    <t>chance_diffusible(35)</t>
+  </si>
+  <si>
+    <t>Chance of "Red room" being trapped</t>
+  </si>
+  <si>
+    <t>Border Crossing: Mexico</t>
+  </si>
+  <si>
+    <t>Border Crossing: Arizona</t>
+  </si>
+  <si>
+    <t>102290</t>
+  </si>
+  <si>
+    <t>random_spawn_camera_npc</t>
+  </si>
+  <si>
+    <t>102284</t>
+  </si>
+  <si>
+    <t>enemy_camera_guard_mexico001</t>
+  </si>
+  <si>
+    <t>enemy_camera_guard_mexico002</t>
   </si>
 </sst>
 </file>
@@ -16190,17 +16259,17 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -18902,7 +18971,7 @@
         <v>4055</v>
       </c>
       <c r="F85" s="2"/>
-      <c r="G85" s="93"/>
+      <c r="G85" s="95"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="15" t="s">
@@ -18921,7 +18990,7 @@
         <v>4056</v>
       </c>
       <c r="F86" s="2"/>
-      <c r="G86" s="93"/>
+      <c r="G86" s="95"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="15" t="s">
@@ -18940,7 +19009,7 @@
         <v>4056</v>
       </c>
       <c r="F87" s="2"/>
-      <c r="G87" s="93"/>
+      <c r="G87" s="95"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="102" t="s">
@@ -18991,7 +19060,7 @@
       </c>
       <c r="E90" s="2"/>
       <c r="F90" s="2"/>
-      <c r="G90" s="93"/>
+      <c r="G90" s="95"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="15" t="s">
@@ -19008,7 +19077,7 @@
       </c>
       <c r="E91" s="2"/>
       <c r="F91" s="2"/>
-      <c r="G91" s="93"/>
+      <c r="G91" s="95"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="15" t="s">
@@ -19025,7 +19094,7 @@
       </c>
       <c r="E92" s="2"/>
       <c r="F92" s="2"/>
-      <c r="G92" s="93"/>
+      <c r="G92" s="95"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="15" t="s">
@@ -19042,7 +19111,7 @@
       </c>
       <c r="E93" s="2"/>
       <c r="F93" s="2"/>
-      <c r="G93" s="93"/>
+      <c r="G93" s="95"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
@@ -19059,7 +19128,7 @@
       </c>
       <c r="E94" s="2"/>
       <c r="F94" s="2"/>
-      <c r="G94" s="93"/>
+      <c r="G94" s="95"/>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="15" t="s">
@@ -19076,7 +19145,7 @@
       </c>
       <c r="E95" s="2"/>
       <c r="F95" s="2"/>
-      <c r="G95" s="93"/>
+      <c r="G95" s="95"/>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="102" t="s">
@@ -19125,7 +19194,7 @@
       </c>
       <c r="E98" s="2"/>
       <c r="F98" s="2"/>
-      <c r="G98" s="92"/>
+      <c r="G98" s="94"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="15" t="s">
@@ -19142,7 +19211,7 @@
       </c>
       <c r="E99" s="2"/>
       <c r="F99" s="2"/>
-      <c r="G99" s="93"/>
+      <c r="G99" s="95"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="15" t="s">
@@ -19159,7 +19228,7 @@
       </c>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
-      <c r="G100" s="93"/>
+      <c r="G100" s="95"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="15" t="s">
@@ -19176,7 +19245,7 @@
       </c>
       <c r="E101" s="2"/>
       <c r="F101" s="2"/>
-      <c r="G101" s="93"/>
+      <c r="G101" s="95"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="15" t="s">
@@ -19193,7 +19262,7 @@
       </c>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
-      <c r="G102" s="93"/>
+      <c r="G102" s="95"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
@@ -19210,7 +19279,7 @@
       </c>
       <c r="E103" s="2"/>
       <c r="F103" s="2"/>
-      <c r="G103" s="93"/>
+      <c r="G103" s="95"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="15" t="s">
@@ -19227,7 +19296,7 @@
       </c>
       <c r="E104" s="2"/>
       <c r="F104" s="2"/>
-      <c r="G104" s="93"/>
+      <c r="G104" s="95"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="15" t="s">
@@ -19244,7 +19313,7 @@
       </c>
       <c r="E105" s="2"/>
       <c r="F105" s="2"/>
-      <c r="G105" s="93"/>
+      <c r="G105" s="95"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="15" t="s">
@@ -19261,7 +19330,7 @@
       </c>
       <c r="E106" s="2"/>
       <c r="F106" s="2"/>
-      <c r="G106" s="93"/>
+      <c r="G106" s="95"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="15" t="s">
@@ -19278,7 +19347,7 @@
       </c>
       <c r="E107" s="2"/>
       <c r="F107" s="2"/>
-      <c r="G107" s="93"/>
+      <c r="G107" s="95"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="15" t="s">
@@ -19295,7 +19364,7 @@
       </c>
       <c r="E108" s="2"/>
       <c r="F108" s="2"/>
-      <c r="G108" s="93"/>
+      <c r="G108" s="95"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="15" t="s">
@@ -19312,7 +19381,7 @@
       </c>
       <c r="E109" s="2"/>
       <c r="F109" s="2"/>
-      <c r="G109" s="93"/>
+      <c r="G109" s="95"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="102" t="s">
@@ -19363,7 +19432,7 @@
         <v>4046</v>
       </c>
       <c r="F112" s="2"/>
-      <c r="G112" s="93"/>
+      <c r="G112" s="95"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
@@ -19382,7 +19451,7 @@
         <v>4047</v>
       </c>
       <c r="F113" s="2"/>
-      <c r="G113" s="93"/>
+      <c r="G113" s="95"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="15" t="s">
@@ -19401,7 +19470,7 @@
         <v>4048</v>
       </c>
       <c r="F114" s="2"/>
-      <c r="G114" s="93"/>
+      <c r="G114" s="95"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
@@ -19420,7 +19489,7 @@
         <v>4049</v>
       </c>
       <c r="F115" s="2"/>
-      <c r="G115" s="93"/>
+      <c r="G115" s="95"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="90" t="s">
@@ -21721,7 +21790,7 @@
         <v>3620</v>
       </c>
       <c r="F236" s="2"/>
-      <c r="G236" s="92" t="s">
+      <c r="G236" s="94" t="s">
         <v>3076</v>
       </c>
     </row>
@@ -21742,7 +21811,7 @@
         <v>3621</v>
       </c>
       <c r="F237" s="2"/>
-      <c r="G237" s="93"/>
+      <c r="G237" s="95"/>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="15" t="s">
@@ -21761,7 +21830,7 @@
         <v>3622</v>
       </c>
       <c r="F238" s="2"/>
-      <c r="G238" s="93"/>
+      <c r="G238" s="95"/>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="15" t="s">
@@ -21780,7 +21849,7 @@
         <v>3623</v>
       </c>
       <c r="F239" s="2"/>
-      <c r="G239" s="93"/>
+      <c r="G239" s="95"/>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="15" t="s">
@@ -21799,7 +21868,7 @@
         <v>3624</v>
       </c>
       <c r="F240" s="2"/>
-      <c r="G240" s="93"/>
+      <c r="G240" s="95"/>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="15" t="s">
@@ -21818,7 +21887,7 @@
         <v>3625</v>
       </c>
       <c r="F241" s="2"/>
-      <c r="G241" s="93"/>
+      <c r="G241" s="95"/>
     </row>
     <row r="242" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A242" s="15" t="s">
@@ -21837,7 +21906,7 @@
         <v>3626</v>
       </c>
       <c r="F242" s="2"/>
-      <c r="G242" s="93"/>
+      <c r="G242" s="95"/>
     </row>
     <row r="243" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A243" s="15" t="s">
@@ -21856,7 +21925,7 @@
         <v>3627</v>
       </c>
       <c r="F243" s="2"/>
-      <c r="G243" s="93"/>
+      <c r="G243" s="95"/>
     </row>
     <row r="244" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A244" s="15" t="s">
@@ -21875,7 +21944,7 @@
         <v>3628</v>
       </c>
       <c r="F244" s="2"/>
-      <c r="G244" s="93"/>
+      <c r="G244" s="95"/>
     </row>
     <row r="245" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A245" s="13" t="s">
@@ -25375,6 +25444,15 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A424:G424"/>
+    <mergeCell ref="A251:G251"/>
+    <mergeCell ref="A143:G143"/>
+    <mergeCell ref="A149:G149"/>
+    <mergeCell ref="A219:G219"/>
+    <mergeCell ref="A256:G256"/>
+    <mergeCell ref="A312:G312"/>
+    <mergeCell ref="A404:G404"/>
+    <mergeCell ref="G236:G244"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A117:G117"/>
@@ -25388,15 +25466,6 @@
     <mergeCell ref="G112:G115"/>
     <mergeCell ref="A83:G83"/>
     <mergeCell ref="G85:G87"/>
-    <mergeCell ref="A424:G424"/>
-    <mergeCell ref="A251:G251"/>
-    <mergeCell ref="A143:G143"/>
-    <mergeCell ref="A149:G149"/>
-    <mergeCell ref="A219:G219"/>
-    <mergeCell ref="A256:G256"/>
-    <mergeCell ref="A312:G312"/>
-    <mergeCell ref="A404:G404"/>
-    <mergeCell ref="G236:G244"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -28723,7 +28792,7 @@
         <v>3086</v>
       </c>
       <c r="F177" s="2"/>
-      <c r="G177" s="92" t="s">
+      <c r="G177" s="94" t="s">
         <v>3092</v>
       </c>
     </row>
@@ -28744,7 +28813,7 @@
         <v>3087</v>
       </c>
       <c r="F178" s="2"/>
-      <c r="G178" s="93"/>
+      <c r="G178" s="95"/>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="12">
@@ -28763,7 +28832,7 @@
         <v>3088</v>
       </c>
       <c r="F179" s="2"/>
-      <c r="G179" s="93"/>
+      <c r="G179" s="95"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="12">
@@ -28782,7 +28851,7 @@
         <v>3089</v>
       </c>
       <c r="F180" s="2"/>
-      <c r="G180" s="93"/>
+      <c r="G180" s="95"/>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="12">
@@ -28801,7 +28870,7 @@
         <v>3090</v>
       </c>
       <c r="F181" s="2"/>
-      <c r="G181" s="93"/>
+      <c r="G181" s="95"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="12">
@@ -28820,7 +28889,7 @@
         <v>3091</v>
       </c>
       <c r="F182" s="2"/>
-      <c r="G182" s="93"/>
+      <c r="G182" s="95"/>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="90" t="s">
@@ -30739,6 +30808,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A237:G237"/>
+    <mergeCell ref="A268:G268"/>
+    <mergeCell ref="A283:G283"/>
+    <mergeCell ref="A226:G226"/>
+    <mergeCell ref="A228:G228"/>
+    <mergeCell ref="A230:G230"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A184:G184"/>
     <mergeCell ref="A193:G193"/>
@@ -30746,12 +30821,6 @@
     <mergeCell ref="A73:G73"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="G177:G182"/>
-    <mergeCell ref="A237:G237"/>
-    <mergeCell ref="A268:G268"/>
-    <mergeCell ref="A283:G283"/>
-    <mergeCell ref="A226:G226"/>
-    <mergeCell ref="A228:G228"/>
-    <mergeCell ref="A230:G230"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A228:G228" location="Bain!A1" display="See &quot;Bain&quot; - Art Gallery" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
@@ -33822,12 +33891,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A55:G55"/>
-    <mergeCell ref="A63:G63"/>
-    <mergeCell ref="A112:G112"/>
-    <mergeCell ref="A107:G107"/>
     <mergeCell ref="A130:G130"/>
     <mergeCell ref="A155:G155"/>
     <mergeCell ref="A159:G159"/>
@@ -33837,6 +33900,12 @@
     <mergeCell ref="A149:G149"/>
     <mergeCell ref="A152:G152"/>
     <mergeCell ref="A157:G157"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A55:G55"/>
+    <mergeCell ref="A63:G63"/>
+    <mergeCell ref="A112:G112"/>
+    <mergeCell ref="A107:G107"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A157:G157" location="Bain!A1" display="See &quot;Bain&quot; - Art Gallery" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
@@ -34282,7 +34351,7 @@
         <v>560</v>
       </c>
       <c r="F21" s="19"/>
-      <c r="G21" s="92" t="s">
+      <c r="G21" s="94" t="s">
         <v>707</v>
       </c>
     </row>
@@ -34303,7 +34372,7 @@
         <v>560</v>
       </c>
       <c r="F22" s="19"/>
-      <c r="G22" s="92"/>
+      <c r="G22" s="94"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -34322,7 +34391,7 @@
         <v>560</v>
       </c>
       <c r="F23" s="19"/>
-      <c r="G23" s="92"/>
+      <c r="G23" s="94"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
@@ -34341,7 +34410,7 @@
         <v>560</v>
       </c>
       <c r="F24" s="19"/>
-      <c r="G24" s="92"/>
+      <c r="G24" s="94"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
@@ -34360,7 +34429,7 @@
         <v>560</v>
       </c>
       <c r="F25" s="19"/>
-      <c r="G25" s="92"/>
+      <c r="G25" s="94"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
@@ -34379,7 +34448,7 @@
         <v>560</v>
       </c>
       <c r="F26" s="19"/>
-      <c r="G26" s="92"/>
+      <c r="G26" s="94"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
@@ -34398,7 +34467,7 @@
         <v>560</v>
       </c>
       <c r="F27" s="19"/>
-      <c r="G27" s="92"/>
+      <c r="G27" s="94"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
@@ -34417,7 +34486,7 @@
         <v>560</v>
       </c>
       <c r="F28" s="19"/>
-      <c r="G28" s="92"/>
+      <c r="G28" s="94"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
@@ -34436,7 +34505,7 @@
         <v>703</v>
       </c>
       <c r="F29" s="2"/>
-      <c r="G29" s="92" t="s">
+      <c r="G29" s="94" t="s">
         <v>706</v>
       </c>
     </row>
@@ -34457,7 +34526,7 @@
         <v>703</v>
       </c>
       <c r="F30" s="2"/>
-      <c r="G30" s="93"/>
+      <c r="G30" s="95"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
@@ -34476,7 +34545,7 @@
         <v>703</v>
       </c>
       <c r="F31" s="2"/>
-      <c r="G31" s="93"/>
+      <c r="G31" s="95"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
@@ -34495,7 +34564,7 @@
         <v>703</v>
       </c>
       <c r="F32" s="2"/>
-      <c r="G32" s="93"/>
+      <c r="G32" s="95"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
@@ -34514,7 +34583,7 @@
         <v>703</v>
       </c>
       <c r="F33" s="2"/>
-      <c r="G33" s="93"/>
+      <c r="G33" s="95"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
@@ -34533,7 +34602,7 @@
         <v>703</v>
       </c>
       <c r="F34" s="2"/>
-      <c r="G34" s="93"/>
+      <c r="G34" s="95"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
@@ -34552,7 +34621,7 @@
         <v>703</v>
       </c>
       <c r="F35" s="2"/>
-      <c r="G35" s="93"/>
+      <c r="G35" s="95"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
@@ -34571,7 +34640,7 @@
         <v>703</v>
       </c>
       <c r="F36" s="2"/>
-      <c r="G36" s="93"/>
+      <c r="G36" s="95"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
@@ -34590,7 +34659,7 @@
         <v>557</v>
       </c>
       <c r="F37" s="2"/>
-      <c r="G37" s="92" t="s">
+      <c r="G37" s="94" t="s">
         <v>704</v>
       </c>
     </row>
@@ -34611,7 +34680,7 @@
         <v>557</v>
       </c>
       <c r="F38" s="2"/>
-      <c r="G38" s="93"/>
+      <c r="G38" s="95"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
@@ -34630,7 +34699,7 @@
         <v>557</v>
       </c>
       <c r="F39" s="2"/>
-      <c r="G39" s="93"/>
+      <c r="G39" s="95"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
@@ -34649,7 +34718,7 @@
         <v>557</v>
       </c>
       <c r="F40" s="2"/>
-      <c r="G40" s="93"/>
+      <c r="G40" s="95"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
@@ -34668,7 +34737,7 @@
         <v>557</v>
       </c>
       <c r="F41" s="2"/>
-      <c r="G41" s="93"/>
+      <c r="G41" s="95"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
@@ -34687,7 +34756,7 @@
         <v>557</v>
       </c>
       <c r="F42" s="2"/>
-      <c r="G42" s="93"/>
+      <c r="G42" s="95"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
@@ -34706,7 +34775,7 @@
         <v>557</v>
       </c>
       <c r="F43" s="2"/>
-      <c r="G43" s="93"/>
+      <c r="G43" s="95"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
@@ -34725,7 +34794,7 @@
         <v>557</v>
       </c>
       <c r="F44" s="2"/>
-      <c r="G44" s="93"/>
+      <c r="G44" s="95"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
@@ -34744,7 +34813,7 @@
         <v>557</v>
       </c>
       <c r="F45" s="2"/>
-      <c r="G45" s="93"/>
+      <c r="G45" s="95"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="15" t="s">
@@ -34763,7 +34832,7 @@
         <v>557</v>
       </c>
       <c r="F46" s="2"/>
-      <c r="G46" s="93"/>
+      <c r="G46" s="95"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
@@ -34782,7 +34851,7 @@
         <v>559</v>
       </c>
       <c r="F47" s="2"/>
-      <c r="G47" s="92" t="s">
+      <c r="G47" s="94" t="s">
         <v>705</v>
       </c>
     </row>
@@ -34803,7 +34872,7 @@
         <v>559</v>
       </c>
       <c r="F48" s="2"/>
-      <c r="G48" s="93"/>
+      <c r="G48" s="95"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
@@ -34822,7 +34891,7 @@
         <v>559</v>
       </c>
       <c r="F49" s="2"/>
-      <c r="G49" s="93"/>
+      <c r="G49" s="95"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="15" t="s">
@@ -34841,7 +34910,7 @@
         <v>559</v>
       </c>
       <c r="F50" s="2"/>
-      <c r="G50" s="93"/>
+      <c r="G50" s="95"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="15" t="s">
@@ -34860,7 +34929,7 @@
         <v>559</v>
       </c>
       <c r="F51" s="2"/>
-      <c r="G51" s="93"/>
+      <c r="G51" s="95"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="15" t="s">
@@ -34879,7 +34948,7 @@
         <v>559</v>
       </c>
       <c r="F52" s="2"/>
-      <c r="G52" s="93"/>
+      <c r="G52" s="95"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
@@ -34898,7 +34967,7 @@
         <v>559</v>
       </c>
       <c r="F53" s="2"/>
-      <c r="G53" s="93"/>
+      <c r="G53" s="95"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
@@ -34917,7 +34986,7 @@
         <v>559</v>
       </c>
       <c r="F54" s="2"/>
-      <c r="G54" s="93"/>
+      <c r="G54" s="95"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
@@ -34936,7 +35005,7 @@
         <v>702</v>
       </c>
       <c r="F55" s="2"/>
-      <c r="G55" s="92" t="s">
+      <c r="G55" s="94" t="s">
         <v>708</v>
       </c>
     </row>
@@ -34957,7 +35026,7 @@
         <v>702</v>
       </c>
       <c r="F56" s="2"/>
-      <c r="G56" s="93"/>
+      <c r="G56" s="95"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="15" t="s">
@@ -34976,7 +35045,7 @@
         <v>702</v>
       </c>
       <c r="F57" s="2"/>
-      <c r="G57" s="93"/>
+      <c r="G57" s="95"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="15" t="s">
@@ -34995,7 +35064,7 @@
         <v>702</v>
       </c>
       <c r="F58" s="2"/>
-      <c r="G58" s="93"/>
+      <c r="G58" s="95"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="15" t="s">
@@ -35014,7 +35083,7 @@
         <v>702</v>
       </c>
       <c r="F59" s="2"/>
-      <c r="G59" s="93"/>
+      <c r="G59" s="95"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="15" t="s">
@@ -35033,7 +35102,7 @@
         <v>702</v>
       </c>
       <c r="F60" s="2"/>
-      <c r="G60" s="93"/>
+      <c r="G60" s="95"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
@@ -35052,7 +35121,7 @@
         <v>702</v>
       </c>
       <c r="F61" s="2"/>
-      <c r="G61" s="93"/>
+      <c r="G61" s="95"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
@@ -35071,7 +35140,7 @@
         <v>702</v>
       </c>
       <c r="F62" s="2"/>
-      <c r="G62" s="93"/>
+      <c r="G62" s="95"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="15" t="s">
@@ -35090,7 +35159,7 @@
         <v>702</v>
       </c>
       <c r="F63" s="2"/>
-      <c r="G63" s="93"/>
+      <c r="G63" s="95"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="15" t="s">
@@ -35109,7 +35178,7 @@
         <v>702</v>
       </c>
       <c r="F64" s="2"/>
-      <c r="G64" s="93"/>
+      <c r="G64" s="95"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
@@ -35128,7 +35197,7 @@
         <v>702</v>
       </c>
       <c r="F65" s="2"/>
-      <c r="G65" s="93"/>
+      <c r="G65" s="95"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="15" t="s">
@@ -35147,7 +35216,7 @@
         <v>702</v>
       </c>
       <c r="F66" s="2"/>
-      <c r="G66" s="93"/>
+      <c r="G66" s="95"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="90" t="s">
@@ -35895,15 +35964,15 @@
       <c r="G104" s="22"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="94" t="s">
+      <c r="A106" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="B106" s="94"/>
-      <c r="C106" s="94"/>
-      <c r="D106" s="94"/>
-      <c r="E106" s="94"/>
-      <c r="F106" s="94"/>
-      <c r="G106" s="94"/>
+      <c r="B106" s="92"/>
+      <c r="C106" s="92"/>
+      <c r="D106" s="92"/>
+      <c r="E106" s="92"/>
+      <c r="F106" s="92"/>
+      <c r="G106" s="92"/>
     </row>
     <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="9" t="s">
@@ -36221,7 +36290,7 @@
         <v>2940</v>
       </c>
       <c r="F122" s="2"/>
-      <c r="G122" s="92" t="s">
+      <c r="G122" s="94" t="s">
         <v>2942</v>
       </c>
     </row>
@@ -36242,7 +36311,7 @@
         <v>2940</v>
       </c>
       <c r="F123" s="2"/>
-      <c r="G123" s="93"/>
+      <c r="G123" s="95"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="12">
@@ -36261,7 +36330,7 @@
         <v>2940</v>
       </c>
       <c r="F124" s="2"/>
-      <c r="G124" s="93"/>
+      <c r="G124" s="95"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="12">
@@ -36280,7 +36349,7 @@
         <v>2940</v>
       </c>
       <c r="F125" s="2"/>
-      <c r="G125" s="93"/>
+      <c r="G125" s="95"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="12">
@@ -36299,7 +36368,7 @@
         <v>2940</v>
       </c>
       <c r="F126" s="2"/>
-      <c r="G126" s="93"/>
+      <c r="G126" s="95"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="12">
@@ -36318,7 +36387,7 @@
         <v>2940</v>
       </c>
       <c r="F127" s="2"/>
-      <c r="G127" s="93"/>
+      <c r="G127" s="95"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="12">
@@ -36337,7 +36406,7 @@
         <v>2940</v>
       </c>
       <c r="F128" s="2"/>
-      <c r="G128" s="93"/>
+      <c r="G128" s="95"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="12">
@@ -36356,7 +36425,7 @@
         <v>2940</v>
       </c>
       <c r="F129" s="2"/>
-      <c r="G129" s="93"/>
+      <c r="G129" s="95"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="12">
@@ -36375,7 +36444,7 @@
         <v>2939</v>
       </c>
       <c r="F130" s="2"/>
-      <c r="G130" s="92" t="s">
+      <c r="G130" s="94" t="s">
         <v>2941</v>
       </c>
     </row>
@@ -36396,7 +36465,7 @@
         <v>2939</v>
       </c>
       <c r="F131" s="2"/>
-      <c r="G131" s="93"/>
+      <c r="G131" s="95"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="12">
@@ -36415,7 +36484,7 @@
         <v>2939</v>
       </c>
       <c r="F132" s="2"/>
-      <c r="G132" s="93"/>
+      <c r="G132" s="95"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="12">
@@ -36434,7 +36503,7 @@
         <v>2939</v>
       </c>
       <c r="F133" s="2"/>
-      <c r="G133" s="93"/>
+      <c r="G133" s="95"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="12">
@@ -36453,7 +36522,7 @@
         <v>2939</v>
       </c>
       <c r="F134" s="2"/>
-      <c r="G134" s="93"/>
+      <c r="G134" s="95"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="12">
@@ -36472,7 +36541,7 @@
         <v>2939</v>
       </c>
       <c r="F135" s="2"/>
-      <c r="G135" s="93"/>
+      <c r="G135" s="95"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="12">
@@ -36491,7 +36560,7 @@
         <v>2939</v>
       </c>
       <c r="F136" s="2"/>
-      <c r="G136" s="93"/>
+      <c r="G136" s="95"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="12">
@@ -36673,15 +36742,15 @@
       <c r="G145" s="3"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A147" s="94" t="s">
+      <c r="A147" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="B147" s="94"/>
-      <c r="C147" s="94"/>
-      <c r="D147" s="94"/>
-      <c r="E147" s="94"/>
-      <c r="F147" s="94"/>
-      <c r="G147" s="94"/>
+      <c r="B147" s="92"/>
+      <c r="C147" s="92"/>
+      <c r="D147" s="92"/>
+      <c r="E147" s="92"/>
+      <c r="F147" s="92"/>
+      <c r="G147" s="92"/>
     </row>
     <row r="148" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="9" t="s">
@@ -37314,15 +37383,15 @@
       <c r="G179" s="2"/>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="94" t="s">
+      <c r="A181" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="B181" s="94"/>
-      <c r="C181" s="94"/>
-      <c r="D181" s="94"/>
-      <c r="E181" s="94"/>
-      <c r="F181" s="94"/>
-      <c r="G181" s="94"/>
+      <c r="B181" s="92"/>
+      <c r="C181" s="92"/>
+      <c r="D181" s="92"/>
+      <c r="E181" s="92"/>
+      <c r="F181" s="92"/>
+      <c r="G181" s="92"/>
     </row>
     <row r="182" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="9" t="s">
@@ -37611,15 +37680,15 @@
       <c r="G195" s="2"/>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A197" s="94" t="s">
+      <c r="A197" s="92" t="s">
         <v>36</v>
       </c>
-      <c r="B197" s="94"/>
-      <c r="C197" s="94"/>
-      <c r="D197" s="94"/>
-      <c r="E197" s="94"/>
-      <c r="F197" s="94"/>
-      <c r="G197" s="94"/>
+      <c r="B197" s="92"/>
+      <c r="C197" s="92"/>
+      <c r="D197" s="92"/>
+      <c r="E197" s="92"/>
+      <c r="F197" s="92"/>
+      <c r="G197" s="92"/>
     </row>
     <row r="198" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="9" t="s">
@@ -37973,15 +38042,15 @@
       <c r="G214" s="2"/>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A216" s="94" t="s">
+      <c r="A216" s="92" t="s">
         <v>37</v>
       </c>
-      <c r="B216" s="94"/>
-      <c r="C216" s="94"/>
-      <c r="D216" s="94"/>
-      <c r="E216" s="94"/>
-      <c r="F216" s="94"/>
-      <c r="G216" s="94"/>
+      <c r="B216" s="92"/>
+      <c r="C216" s="92"/>
+      <c r="D216" s="92"/>
+      <c r="E216" s="92"/>
+      <c r="F216" s="92"/>
+      <c r="G216" s="92"/>
     </row>
     <row r="217" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A217" s="9" t="s">
@@ -38723,15 +38792,15 @@
       <c r="G251" s="2"/>
     </row>
     <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" s="94" t="s">
+      <c r="A253" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="B253" s="94"/>
-      <c r="C253" s="94"/>
-      <c r="D253" s="94"/>
-      <c r="E253" s="94"/>
-      <c r="F253" s="94"/>
-      <c r="G253" s="94"/>
+      <c r="B253" s="92"/>
+      <c r="C253" s="92"/>
+      <c r="D253" s="92"/>
+      <c r="E253" s="92"/>
+      <c r="F253" s="92"/>
+      <c r="G253" s="92"/>
     </row>
     <row r="254" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A254" s="9" t="s">
@@ -39320,15 +39389,15 @@
       <c r="G281" s="2"/>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A283" s="94" t="s">
+      <c r="A283" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="B283" s="94"/>
-      <c r="C283" s="94"/>
-      <c r="D283" s="94"/>
-      <c r="E283" s="94"/>
-      <c r="F283" s="94"/>
-      <c r="G283" s="94"/>
+      <c r="B283" s="92"/>
+      <c r="C283" s="92"/>
+      <c r="D283" s="92"/>
+      <c r="E283" s="92"/>
+      <c r="F283" s="92"/>
+      <c r="G283" s="92"/>
     </row>
     <row r="284" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="9" t="s">
@@ -39516,15 +39585,15 @@
       <c r="G292" s="3"/>
     </row>
     <row r="294" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A294" s="94" t="s">
+      <c r="A294" s="92" t="s">
         <v>40</v>
       </c>
-      <c r="B294" s="94"/>
-      <c r="C294" s="94"/>
-      <c r="D294" s="94"/>
-      <c r="E294" s="94"/>
-      <c r="F294" s="94"/>
-      <c r="G294" s="94"/>
+      <c r="B294" s="92"/>
+      <c r="C294" s="92"/>
+      <c r="D294" s="92"/>
+      <c r="E294" s="92"/>
+      <c r="F294" s="92"/>
+      <c r="G294" s="92"/>
     </row>
     <row r="295" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A295" s="9" t="s">
@@ -39573,15 +39642,15 @@
       </c>
     </row>
     <row r="298" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A298" s="94" t="s">
+      <c r="A298" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="B298" s="94"/>
-      <c r="C298" s="94"/>
-      <c r="D298" s="94"/>
-      <c r="E298" s="94"/>
-      <c r="F298" s="94"/>
-      <c r="G298" s="94"/>
+      <c r="B298" s="92"/>
+      <c r="C298" s="92"/>
+      <c r="D298" s="92"/>
+      <c r="E298" s="92"/>
+      <c r="F298" s="92"/>
+      <c r="G298" s="92"/>
     </row>
     <row r="299" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A299" s="9" t="s">
@@ -39628,15 +39697,15 @@
       <c r="G300" s="6"/>
     </row>
     <row r="302" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A302" s="94" t="s">
+      <c r="A302" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="B302" s="94"/>
-      <c r="C302" s="94"/>
-      <c r="D302" s="94"/>
-      <c r="E302" s="94"/>
-      <c r="F302" s="94"/>
-      <c r="G302" s="94"/>
+      <c r="B302" s="92"/>
+      <c r="C302" s="92"/>
+      <c r="D302" s="92"/>
+      <c r="E302" s="92"/>
+      <c r="F302" s="92"/>
+      <c r="G302" s="92"/>
     </row>
     <row r="303" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A303" s="9" t="s">
@@ -39744,15 +39813,15 @@
       <c r="G307" s="2"/>
     </row>
     <row r="309" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A309" s="94" t="s">
+      <c r="A309" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="B309" s="94"/>
-      <c r="C309" s="94"/>
-      <c r="D309" s="94"/>
-      <c r="E309" s="94"/>
-      <c r="F309" s="94"/>
-      <c r="G309" s="94"/>
+      <c r="B309" s="92"/>
+      <c r="C309" s="92"/>
+      <c r="D309" s="92"/>
+      <c r="E309" s="92"/>
+      <c r="F309" s="92"/>
+      <c r="G309" s="92"/>
     </row>
     <row r="310" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A310" s="9" t="s">
@@ -39858,15 +39927,15 @@
       <c r="G314" s="2"/>
     </row>
     <row r="316" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A316" s="94" t="s">
+      <c r="A316" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="B316" s="94"/>
-      <c r="C316" s="94"/>
-      <c r="D316" s="94"/>
-      <c r="E316" s="94"/>
-      <c r="F316" s="94"/>
-      <c r="G316" s="94"/>
+      <c r="B316" s="92"/>
+      <c r="C316" s="92"/>
+      <c r="D316" s="92"/>
+      <c r="E316" s="92"/>
+      <c r="F316" s="92"/>
+      <c r="G316" s="92"/>
     </row>
     <row r="317" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A317" s="9" t="s">
@@ -40696,15 +40765,15 @@
       <c r="G370" s="2"/>
     </row>
     <row r="371" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A371" s="95" t="s">
+      <c r="A371" s="93" t="s">
         <v>3921</v>
       </c>
-      <c r="B371" s="95"/>
-      <c r="C371" s="95"/>
-      <c r="D371" s="95"/>
-      <c r="E371" s="95"/>
-      <c r="F371" s="95"/>
-      <c r="G371" s="95"/>
+      <c r="B371" s="93"/>
+      <c r="C371" s="93"/>
+      <c r="D371" s="93"/>
+      <c r="E371" s="93"/>
+      <c r="F371" s="93"/>
+      <c r="G371" s="93"/>
     </row>
     <row r="372" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A372" s="45" t="s">
@@ -40811,19 +40880,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A253:G253"/>
-    <mergeCell ref="A216:G216"/>
-    <mergeCell ref="A197:G197"/>
-    <mergeCell ref="A181:G181"/>
-    <mergeCell ref="A147:G147"/>
-    <mergeCell ref="A376:G376"/>
-    <mergeCell ref="A283:G283"/>
-    <mergeCell ref="A294:G294"/>
-    <mergeCell ref="A298:G298"/>
-    <mergeCell ref="A302:G302"/>
-    <mergeCell ref="A309:G309"/>
-    <mergeCell ref="A316:G316"/>
-    <mergeCell ref="A371:G371"/>
     <mergeCell ref="G130:G136"/>
     <mergeCell ref="G122:G129"/>
     <mergeCell ref="A106:G106"/>
@@ -40835,6 +40891,19 @@
     <mergeCell ref="G21:G28"/>
     <mergeCell ref="G29:G36"/>
     <mergeCell ref="G37:G46"/>
+    <mergeCell ref="A376:G376"/>
+    <mergeCell ref="A283:G283"/>
+    <mergeCell ref="A294:G294"/>
+    <mergeCell ref="A298:G298"/>
+    <mergeCell ref="A302:G302"/>
+    <mergeCell ref="A309:G309"/>
+    <mergeCell ref="A316:G316"/>
+    <mergeCell ref="A371:G371"/>
+    <mergeCell ref="A253:G253"/>
+    <mergeCell ref="A216:G216"/>
+    <mergeCell ref="A197:G197"/>
+    <mergeCell ref="A181:G181"/>
+    <mergeCell ref="A147:G147"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -40845,8 +40914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G158"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="A123" sqref="A123:G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48230,16 +48299,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A182:G182"/>
+    <mergeCell ref="A133:G133"/>
+    <mergeCell ref="A143:G143"/>
+    <mergeCell ref="A163:G163"/>
+    <mergeCell ref="A175:G175"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="A129:G129"/>
     <mergeCell ref="A131:G131"/>
-    <mergeCell ref="A182:G182"/>
-    <mergeCell ref="A133:G133"/>
-    <mergeCell ref="A143:G143"/>
-    <mergeCell ref="A163:G163"/>
-    <mergeCell ref="A175:G175"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A131:G131" location="Bain!A1" display="See &quot;Bain&quot; - Bank Heist(s)" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
@@ -48251,10 +48320,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:G130"/>
+  <dimension ref="A1:G147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="I122" sqref="I122"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="F150" sqref="F150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48280,7 +48349,7 @@
       <c r="G1" s="100"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="92" t="s">
         <v>923</v>
       </c>
       <c r="B2" s="90"/>
@@ -49726,7 +49795,7 @@
       <c r="G73" s="2"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="94" t="s">
+      <c r="A75" s="92" t="s">
         <v>924</v>
       </c>
       <c r="B75" s="90"/>
@@ -49760,7 +49829,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="94" t="s">
+      <c r="A78" s="92" t="s">
         <v>4242</v>
       </c>
       <c r="B78" s="90"/>
@@ -50654,8 +50723,287 @@
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
     </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="92" t="s">
+        <v>4301</v>
+      </c>
+      <c r="B132" s="90"/>
+      <c r="C132" s="90"/>
+      <c r="D132" s="90"/>
+      <c r="E132" s="90"/>
+      <c r="F132" s="90"/>
+      <c r="G132" s="90"/>
+    </row>
+    <row r="133" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C133" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F133" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G133" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="34" t="s">
+        <v>1687</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>4298</v>
+      </c>
+      <c r="C134" s="10" t="s">
+        <v>3810</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E134" s="6" t="s">
+        <v>4299</v>
+      </c>
+      <c r="F134" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="G134" s="6"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>4294</v>
+      </c>
+      <c r="C135" s="7" t="s">
+        <v>4293</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>4295</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G135" s="3"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="B136" s="4">
+        <v>1</v>
+      </c>
+      <c r="C136" s="15" t="s">
+        <v>4296</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="B137" s="4">
+        <v>2</v>
+      </c>
+      <c r="C137" s="15" t="s">
+        <v>4297</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E137" s="2"/>
+      <c r="F137" s="2"/>
+      <c r="G137" s="2"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="92" t="s">
+        <v>4300</v>
+      </c>
+      <c r="B139" s="90"/>
+      <c r="C139" s="90"/>
+      <c r="D139" s="90"/>
+      <c r="E139" s="90"/>
+      <c r="F139" s="90"/>
+      <c r="G139" s="90"/>
+    </row>
+    <row r="140" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A140" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C140" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="G140" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B141" s="3" t="s">
+        <v>4285</v>
+      </c>
+      <c r="C141" s="7" t="s">
+        <v>4284</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>4189</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G141" s="3"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>4286</v>
+      </c>
+      <c r="C142" s="15" t="s">
+        <v>4201</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>4287</v>
+      </c>
+      <c r="F142" s="2"/>
+      <c r="G142" s="2"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>4289</v>
+      </c>
+      <c r="C143" s="15" t="s">
+        <v>4288</v>
+      </c>
+      <c r="D143" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>4290</v>
+      </c>
+      <c r="F143" s="2"/>
+      <c r="G143" s="2"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="15" t="s">
+        <v>442</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>4291</v>
+      </c>
+      <c r="C144" s="15" t="s">
+        <v>4125</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>4292</v>
+      </c>
+      <c r="F144" s="2"/>
+      <c r="G144" s="2"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>4303</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>4302</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>4295</v>
+      </c>
+      <c r="F145" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G145" s="3"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>4306</v>
+      </c>
+      <c r="C146" s="15" t="s">
+        <v>1637</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E146" s="2"/>
+      <c r="F146" s="2"/>
+      <c r="G146" s="2"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>4305</v>
+      </c>
+      <c r="C147" s="15" t="s">
+        <v>4304</v>
+      </c>
+      <c r="D147" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E147" s="2"/>
+      <c r="F147" s="2"/>
+      <c r="G147" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
+    <mergeCell ref="A132:G132"/>
+    <mergeCell ref="A139:G139"/>
     <mergeCell ref="A78:G78"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>

</xml_diff>